<commit_message>
Can print from and edit _ratio_table
</commit_message>
<xml_diff>
--- a/Mk5/OV5640/TryingToMakeSense.xlsx
+++ b/Mk5/OV5640/TryingToMakeSense.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gibbens\Documents\Arduino\EyeBolt\Mk5\OV5640\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D80CC55D-A2FD-4E77-ACB7-3ABB5DFE5988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F94C05-8D28-416E-8D6B-B1600D99D255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26505" yWindow="8265" windowWidth="31035" windowHeight="23535" xr2:uid="{63198A25-5996-46E9-907C-AF803957DBE4}"/>
+    <workbookView xWindow="12510" yWindow="4830" windowWidth="21675" windowHeight="23535" xr2:uid="{63198A25-5996-46E9-907C-AF803957DBE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="128">
   <si>
     <t>physical</t>
   </si>
@@ -183,13 +184,265 @@
   </si>
   <si>
     <t>9x16</t>
+  </si>
+  <si>
+    <t>self._binning</t>
+  </si>
+  <si>
+    <t>self._flip_x</t>
+  </si>
+  <si>
+    <t>self._flip_y</t>
+  </si>
+  <si>
+    <t>self._h</t>
+  </si>
+  <si>
+    <t>self._imagecapture</t>
+  </si>
+  <si>
+    <t>self._imagecapture.capture()</t>
+  </si>
+  <si>
+    <t>self._imagecapture.deinit()</t>
+  </si>
+  <si>
+    <t>self._mclk_pwm.deinit()</t>
+  </si>
+  <si>
+    <t>self._mclk_pwm.frequency self._mclk_pwm else None</t>
+  </si>
+  <si>
+    <t>self._reset</t>
+  </si>
+  <si>
+    <t>self._reset.deinit()</t>
+  </si>
+  <si>
+    <t>self._reset.switch_to_output</t>
+  </si>
+  <si>
+    <t>self._set_colorspace()</t>
+  </si>
+  <si>
+    <t>self._set_image_options()</t>
+  </si>
+  <si>
+    <t>self._set_size_and_colorspace()</t>
+  </si>
+  <si>
+    <t>self._shutdown.deinit()</t>
+  </si>
+  <si>
+    <t>self._shutdown.switch_to_output(False)</t>
+  </si>
+  <si>
+    <t>self._shutdown:</t>
+  </si>
+  <si>
+    <t>self._size</t>
+  </si>
+  <si>
+    <t>self._test_pattern</t>
+  </si>
+  <si>
+    <t>self._w</t>
+  </si>
+  <si>
+    <t>self._white_balance</t>
+  </si>
+  <si>
+    <t>Seems to only be set to None</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Changed within _set_size_and_colorspace()</t>
+  </si>
+  <si>
+    <t>self._colorspace</t>
+  </si>
+  <si>
+    <t>OV5640_COLOR_RGB</t>
+  </si>
+  <si>
+    <t>Enum - defaults to RGB</t>
+  </si>
+  <si>
+    <t>self._effect</t>
+  </si>
+  <si>
+    <t>OV5640_SPECIAL_EFFECT_</t>
+  </si>
+  <si>
+    <t>Enum for special effects</t>
+  </si>
+  <si>
+    <t>self._bank</t>
+  </si>
+  <si>
+    <t>self._ev</t>
+  </si>
+  <si>
+    <t>self._i2c_device</t>
+  </si>
+  <si>
+    <t>self._mclk_pwm</t>
+  </si>
+  <si>
+    <t>self._mclk_pwm.duty_cycle</t>
+  </si>
+  <si>
+    <t>self._saturation</t>
+  </si>
+  <si>
+    <t>self._scale</t>
+  </si>
+  <si>
+    <t>self._shutdown</t>
+  </si>
+  <si>
+    <t>Sensor exposure (-4 to 4)</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>In _set_size_and_colorspace() this is set from values within _resolution_info[] table</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t># Initialize the master clock</t>
+  </si>
+  <si>
+    <t>self._write_register(0x5381 + offset, reg_value)</t>
+  </si>
+  <si>
+    <t>Set and used within _set_size_and_colorspace()</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Use ._colorspace to lookup into _ov5640_color_settings[] table</t>
+  </si>
+  <si>
+    <t>Uses loads of flip/binning/colourspace values to set registers - doesn't call other methods</t>
+  </si>
+  <si>
+    <t>self._set_pll</t>
+  </si>
+  <si>
+    <t>This sets a lot of hardcode registers</t>
+  </si>
+  <si>
+    <t>This is the business. I think some of the setters here trigger other methods</t>
+  </si>
+  <si>
+    <r>
+      <t>OV5640_SIZE_QQVGA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFE6EDF3"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <t>Setter calls self._set_size_and_colorspace()</t>
+  </si>
+  <si>
+    <t>Defaults to Auto</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Property?</t>
+  </si>
+  <si>
+    <t>colorspace</t>
+  </si>
+  <si>
+    <t>effect</t>
+  </si>
+  <si>
+    <t>exposure_value</t>
+  </si>
+  <si>
+    <t>flip_x</t>
+  </si>
+  <si>
+    <t>flip_y</t>
+  </si>
+  <si>
+    <t>saturation</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>test_pattern</t>
+  </si>
+  <si>
+    <t>white_balance</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>mclk_frequency</t>
+  </si>
+  <si>
+    <t>The frequency of the master clock to generate</t>
+  </si>
+  <si>
+    <t>Pixels</t>
+  </si>
+  <si>
+    <t>bytes</t>
+  </si>
+  <si>
+    <t>kb</t>
+  </si>
+  <si>
+    <t>I want the middle third of the screen</t>
+  </si>
+  <si>
+    <t>available pixels</t>
+  </si>
+  <si>
+    <t>18x19</t>
+  </si>
+  <si>
+    <t>19x18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +465,72 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFE6EDF3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,18 +549,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -553,16 +909,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E851C2E4-06D1-481A-8E90-4AC83D3E53DA}">
-  <dimension ref="A3:U37"/>
+  <dimension ref="A3:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23:V31"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I82" sqref="I82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1203,6 +1560,818 @@
         <v>34</v>
       </c>
     </row>
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G41" s="12"/>
+    </row>
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F46" s="13">
+        <v>24</v>
+      </c>
+      <c r="G46">
+        <f>F44*F45</f>
+        <v>3686400</v>
+      </c>
+      <c r="H46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G47" s="14">
+        <f>G46/F46</f>
+        <v>153600</v>
+      </c>
+      <c r="H47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G48" s="14">
+        <f>G47/1024</f>
+        <v>150</v>
+      </c>
+      <c r="H48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G49" s="14"/>
+      <c r="H49" s="16">
+        <f>G47/2</f>
+        <v>76800</v>
+      </c>
+      <c r="I49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I50" s="14">
+        <f>J54-H49</f>
+        <v>-76800</v>
+      </c>
+    </row>
+    <row r="51" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H52" s="15">
+        <f>950/2560</f>
+        <v>0.37109375</v>
+      </c>
+      <c r="I52" s="15">
+        <f>950/1440</f>
+        <v>0.65972222222222221</v>
+      </c>
+    </row>
+    <row r="54" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>900</v>
+      </c>
+      <c r="I54">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="56" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>270</v>
+      </c>
+      <c r="I56">
+        <v>270</v>
+      </c>
+      <c r="J56">
+        <f>I56*H56</f>
+        <v>72900</v>
+      </c>
+    </row>
+    <row r="58" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>850</v>
+      </c>
+      <c r="I58">
+        <v>950</v>
+      </c>
+      <c r="J58">
+        <f>SUM(H58:I58)</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="59" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>118</v>
+      </c>
+      <c r="G59">
+        <v>950</v>
+      </c>
+      <c r="H59">
+        <f>(G59/950)*I59</f>
+        <v>285</v>
+      </c>
+      <c r="I59">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="60" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>117</v>
+      </c>
+      <c r="G60">
+        <v>900</v>
+      </c>
+      <c r="H60">
+        <f>(G60/950)*I59</f>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="61" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <f>G59/50</f>
+        <v>19</v>
+      </c>
+      <c r="H61">
+        <f>H60*H59</f>
+        <v>76950</v>
+      </c>
+      <c r="I61" s="16">
+        <f>H49-H61</f>
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="62" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G62" s="14">
+        <f>G60/50</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <f>H64/4*3</f>
+        <v>1920</v>
+      </c>
+      <c r="H64">
+        <v>2560</v>
+      </c>
+      <c r="I64">
+        <v>1920</v>
+      </c>
+      <c r="J64" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <f>H65/3*2</f>
+        <v>1706.6666666666667</v>
+      </c>
+      <c r="H65">
+        <v>2560</v>
+      </c>
+      <c r="I65">
+        <v>1704</v>
+      </c>
+      <c r="J65" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H66">
+        <v>2560</v>
+      </c>
+      <c r="I66">
+        <v>1600</v>
+      </c>
+      <c r="J66" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H67">
+        <v>2560</v>
+      </c>
+      <c r="I67">
+        <v>1536</v>
+      </c>
+      <c r="J67" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H68">
+        <v>2560</v>
+      </c>
+      <c r="I68">
+        <v>1440</v>
+      </c>
+      <c r="J68" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H69">
+        <v>2560</v>
+      </c>
+      <c r="I69">
+        <v>1080</v>
+      </c>
+      <c r="J69" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H70">
+        <v>2400</v>
+      </c>
+      <c r="I70">
+        <v>1920</v>
+      </c>
+      <c r="J70" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H71">
+        <v>1920</v>
+      </c>
+      <c r="I71">
+        <v>1920</v>
+      </c>
+      <c r="J71" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H72">
+        <v>1088</v>
+      </c>
+      <c r="I72">
+        <v>1920</v>
+      </c>
+      <c r="J72" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H73" s="17">
+        <v>1820</v>
+      </c>
+      <c r="I73" s="17">
+        <v>1920</v>
+      </c>
+      <c r="J73" s="17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H74">
+        <v>950</v>
+      </c>
+      <c r="I74">
+        <v>900</v>
+      </c>
+      <c r="J74" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="H75" s="2">
+        <v>2650</v>
+      </c>
+      <c r="I75" s="2">
+        <v>1820</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>1536</v>
+      </c>
+      <c r="I79">
+        <v>1584</v>
+      </c>
+      <c r="K79">
+        <f>I79-F79</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>2560</v>
+      </c>
+      <c r="F80">
+        <v>1440</v>
+      </c>
+      <c r="H80">
+        <v>2844</v>
+      </c>
+      <c r="I80">
+        <v>1488</v>
+      </c>
+      <c r="J80">
+        <f>H80-E80</f>
+        <v>284</v>
+      </c>
+      <c r="K80">
+        <f>I80-F80</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>2560</v>
+      </c>
+      <c r="F81">
+        <v>1080</v>
+      </c>
+      <c r="H81">
+        <v>2844</v>
+      </c>
+      <c r="I81">
+        <v>1128</v>
+      </c>
+      <c r="J81">
+        <f>H81-E81</f>
+        <v>284</v>
+      </c>
+      <c r="K81">
+        <f>I81-F81</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="82" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <v>1820</v>
+      </c>
+      <c r="I82">
+        <f>F82+48</f>
+        <v>1868</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE00EBC-9BDF-4691-A203-E98EA342C2A4}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
going to change my_camera_changeSize to run altered size on start-up
</commit_message>
<xml_diff>
--- a/Mk5/OV5640/TryingToMakeSense.xlsx
+++ b/Mk5/OV5640/TryingToMakeSense.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gibbens\Documents\Arduino\EyeBolt\Mk5\OV5640\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F94C05-8D28-416E-8D6B-B1600D99D255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98557CE-2636-4661-8F0F-DF263585B6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="4830" windowWidth="21675" windowHeight="23535" xr2:uid="{63198A25-5996-46E9-907C-AF803957DBE4}"/>
+    <workbookView xWindow="16365" yWindow="13920" windowWidth="21675" windowHeight="13830" xr2:uid="{63198A25-5996-46E9-907C-AF803957DBE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="130">
   <si>
     <t>physical</t>
   </si>
@@ -433,6 +433,12 @@
   <si>
     <t>19x18</t>
   </si>
+  <si>
+    <t>0B</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
 </sst>
 </file>
 
@@ -440,7 +446,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -591,7 +597,7 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -909,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E851C2E4-06D1-481A-8E90-4AC83D3E53DA}">
-  <dimension ref="A3:U82"/>
+  <dimension ref="A3:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I82" sqref="I82"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1728,7 +1734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G65">
         <f>H65/3*2</f>
         <v>1706.6666666666667</v>
@@ -1743,7 +1749,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H66">
         <v>2560</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H67">
         <v>2560</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H68">
         <v>2560</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H69">
         <v>2560</v>
       </c>
@@ -1787,7 +1793,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H70">
         <v>2400</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H71">
         <v>1920</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H72">
         <v>1088</v>
       </c>
@@ -1820,7 +1826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H73" s="17">
         <v>1820</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="74" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H74">
         <v>950</v>
       </c>
@@ -1842,7 +1848,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H75" s="2">
         <v>2650</v>
       </c>
@@ -1853,7 +1859,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2060</v>
+      </c>
+      <c r="B79" t="e">
+        <f>DEC2BIN(A79,16)</f>
+        <v>#NUM!</v>
+      </c>
       <c r="F79">
         <v>1536</v>
       </c>
@@ -1865,7 +1878,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="80" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>984</v>
+      </c>
+      <c r="B80" t="e">
+        <f>DEC2BIN(A80,32)</f>
+        <v>#NUM!</v>
+      </c>
       <c r="E80">
         <v>2560</v>
       </c>
@@ -1887,7 +1907,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E81">
         <v>2560</v>
       </c>
@@ -1909,13 +1929,99 @@
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F82">
         <v>1820</v>
       </c>
       <c r="I82">
         <f>F82+48</f>
         <v>1868</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" t="str">
+        <f>HEX2BIN(A84)</f>
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>129</v>
+      </c>
+      <c r="B85" t="str">
+        <f>HEX2BIN(A85)</f>
+        <v>11100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <v>2560</v>
+      </c>
+      <c r="E87">
+        <v>1920</v>
+      </c>
+      <c r="F87">
+        <v>320</v>
+      </c>
+      <c r="G87">
+        <v>2543</v>
+      </c>
+      <c r="H87">
+        <v>31</v>
+      </c>
+      <c r="I87">
+        <v>2684</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <v>1440</v>
+      </c>
+      <c r="E88">
+        <v>1920</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>1951</v>
+      </c>
+      <c r="H88">
+        <v>16</v>
+      </c>
+      <c r="I88">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <v>2592</v>
+      </c>
+      <c r="E92">
+        <v>2684</v>
+      </c>
+      <c r="F92">
+        <f>E92-D92</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <v>1944</v>
+      </c>
+      <c r="E93">
+        <v>1968</v>
+      </c>
+      <c r="F93">
+        <f>E93-D93</f>
+        <v>24</v>
+      </c>
+      <c r="G93">
+        <f>F93/2</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>